<commit_message>
Purchase temp related issue solution
</commit_message>
<xml_diff>
--- a/6_Inventory_Management/purchase/Purchase temp.xlsx
+++ b/6_Inventory_Management/purchase/Purchase temp.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repos\VBA_Programming\6_Inventory_Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\VBA_Programming\6_Inventory_Management\purchase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B0BAB1-26FB-49B4-9A99-AC72EED84451}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4590"/>
   </bookViews>
   <sheets>
     <sheet name="MasterSheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,12 +29,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tracey.neilson</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -157,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -261,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -355,7 +356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{75057253-89F5-467F-AAA6-92A7378C82C5}">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -449,7 +450,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -553,7 +554,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -681,7 +682,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -804,7 +805,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -934,7 +935,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
   <si>
     <t>Stock Code</t>
   </si>
@@ -1035,48 +1036,6 @@
     <t>AG MIX 1x6</t>
   </si>
   <si>
-    <t>AG10</t>
-  </si>
-  <si>
-    <t>AG METRO MILAN 25GX12</t>
-  </si>
-  <si>
-    <t>AG23</t>
-  </si>
-  <si>
-    <t>AG THREE IN ONE 25GX12</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>BDM SARSON KA SAAG TIN 800GX12</t>
-  </si>
-  <si>
-    <t>HD67</t>
-  </si>
-  <si>
-    <t>HRR SARSOON KA SAAG X 40</t>
-  </si>
-  <si>
-    <t>BG9</t>
-  </si>
-  <si>
-    <t>BG PUNJABI MIX 400G X 12</t>
-  </si>
-  <si>
-    <t>A92</t>
-  </si>
-  <si>
-    <t>BOMBAY SUPARI 48 PACKETS</t>
-  </si>
-  <si>
-    <t>W73</t>
-  </si>
-  <si>
-    <t>WSA FAN STAND 20"INCHX1</t>
-  </si>
-  <si>
     <t>SF17</t>
   </si>
   <si>
@@ -1107,23 +1066,29 @@
     <t>TRS GINGER PWD 400GX10  *offerta*</t>
   </si>
   <si>
-    <t>Expiry Date</t>
+    <t>EXPIRE Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1145,10 +1110,11 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1195,29 +1161,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1309,23 +1270,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1361,23 +1305,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1553,13 +1480,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1578,17 +1505,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>57</v>
+      <c r="D1" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>8</v>
@@ -1610,866 +1537,611 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="8">
         <v>43830</v>
       </c>
       <c r="D2" s="8">
         <v>43554</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="9">
         <v>12</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <v>10</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>43830</v>
       </c>
       <c r="D3" s="8">
         <v>43827</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="9">
         <v>14</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
         <v>10</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>43830</v>
       </c>
       <c r="D4" s="8">
         <v>43827</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="9">
         <v>41</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>10</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>43830</v>
       </c>
       <c r="D5" s="8">
         <v>43827</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="9">
         <v>1</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <v>10</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>43830</v>
       </c>
       <c r="D6" s="8">
         <v>43827</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="9">
         <v>1</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>10</v>
       </c>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="8">
         <v>43830</v>
       </c>
       <c r="D7" s="8">
         <v>43827</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="9">
         <v>48</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>10</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="8">
         <v>43830</v>
       </c>
       <c r="D8" s="8">
         <v>43827</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="9">
         <v>14</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>10</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="8">
         <v>43830</v>
       </c>
       <c r="D9" s="8">
         <v>43827</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="9">
         <v>41</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <v>10</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="8">
         <v>43830</v>
       </c>
       <c r="D10" s="8">
         <v>43827</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="9">
         <v>8</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <v>10</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="8">
         <v>43830</v>
       </c>
       <c r="D11" s="8">
         <v>43827</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="9">
         <v>98</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>10</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="8">
         <v>43830</v>
       </c>
       <c r="D12" s="8">
         <v>43827</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="9">
         <v>31</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <v>10</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="8">
         <v>43830</v>
       </c>
       <c r="D13" s="8">
         <v>43827</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="9">
         <v>2.6666666666666701</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <v>10</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="8">
         <v>43830</v>
       </c>
       <c r="D14" s="8">
         <v>43827</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="9">
         <v>10</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="6">
         <v>10</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="8">
         <v>43830</v>
       </c>
       <c r="D15" s="8">
         <v>43827</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="9">
         <v>68</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="6">
         <v>10</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="8">
         <v>43830</v>
       </c>
       <c r="D16" s="8">
-        <v>43827</v>
-      </c>
-      <c r="E16" s="9" t="s">
+        <v>43828</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="6">
-        <v>8</v>
-      </c>
-      <c r="H16" s="7">
+      <c r="G16" s="9">
+        <v>13</v>
+      </c>
+      <c r="H16" s="6">
         <v>10</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="10">
+      <c r="A17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="8">
         <v>43830</v>
       </c>
       <c r="D17" s="8">
-        <v>43827</v>
-      </c>
-      <c r="E17" s="9" t="s">
+        <v>43828</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="6">
-        <v>25</v>
-      </c>
-      <c r="H17" s="7">
+      <c r="G17" s="9">
+        <v>2</v>
+      </c>
+      <c r="H17" s="6">
         <v>10</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="10">
+      <c r="A18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="8">
         <v>43830</v>
       </c>
       <c r="D18" s="8">
         <v>43828</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="6">
-        <v>1</v>
-      </c>
-      <c r="H18" s="7">
+      <c r="G18" s="9">
+        <v>42</v>
+      </c>
+      <c r="H18" s="6">
         <v>10</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="10">
+      <c r="A19" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="8">
         <v>43830</v>
       </c>
       <c r="D19" s="8">
-        <v>43828</v>
-      </c>
-      <c r="E19" s="9" t="s">
+        <v>43830</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="6">
-        <v>1</v>
-      </c>
-      <c r="H19" s="7">
+      <c r="G19" s="9">
+        <v>3</v>
+      </c>
+      <c r="H19" s="6">
         <v>10</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="8">
         <v>43830</v>
       </c>
       <c r="D20" s="8">
-        <v>43828</v>
-      </c>
-      <c r="E20" s="9" t="s">
+        <v>43860</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="H20" s="7">
+      <c r="G20" s="9">
+        <v>13</v>
+      </c>
+      <c r="H20" s="6">
         <v>10</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="8">
         <v>43830</v>
       </c>
       <c r="D21" s="8">
-        <v>43828</v>
-      </c>
-      <c r="E21" s="9" t="s">
+        <v>43860</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="6">
-        <v>0.91666666666666596</v>
-      </c>
-      <c r="H21" s="7">
+      <c r="G21" s="9">
+        <v>20</v>
+      </c>
+      <c r="H21" s="6">
         <v>10</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="10">
-        <v>43830</v>
-      </c>
-      <c r="D22" s="8">
-        <v>43828</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" s="6">
-        <v>1</v>
-      </c>
-      <c r="H22" s="7">
-        <v>10</v>
-      </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="10">
-        <v>43830</v>
-      </c>
-      <c r="D23" s="8">
-        <v>43828</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="6">
-        <v>1</v>
-      </c>
-      <c r="H23" s="7">
-        <v>10</v>
-      </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="10">
-        <v>43830</v>
-      </c>
-      <c r="D24" s="8">
-        <v>43828</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="6">
-        <v>15</v>
-      </c>
-      <c r="H24" s="7">
-        <v>10</v>
-      </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="10">
-        <v>43830</v>
-      </c>
-      <c r="D25" s="8">
-        <v>43828</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" s="6">
-        <v>13</v>
-      </c>
-      <c r="H25" s="7">
-        <v>10</v>
-      </c>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="10">
-        <v>43830</v>
-      </c>
-      <c r="D26" s="8">
-        <v>43828</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="6">
-        <v>2</v>
-      </c>
-      <c r="H26" s="7">
-        <v>10</v>
-      </c>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="10">
-        <v>43830</v>
-      </c>
-      <c r="D27" s="8">
-        <v>43828</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="6">
-        <v>42</v>
-      </c>
-      <c r="H27" s="7">
-        <v>10</v>
-      </c>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="10">
-        <v>43830</v>
-      </c>
-      <c r="D28" s="8">
-        <v>43830</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G28" s="6">
-        <v>3</v>
-      </c>
-      <c r="H28" s="7">
-        <v>10</v>
-      </c>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="10">
-        <v>43830</v>
-      </c>
-      <c r="D29" s="8">
-        <v>43860</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29" s="6">
-        <v>13</v>
-      </c>
-      <c r="H29" s="7">
-        <v>10</v>
-      </c>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="10">
-        <v>43830</v>
-      </c>
-      <c r="D30" s="8">
-        <v>43860</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="6">
-        <v>20</v>
-      </c>
-      <c r="H30" s="7">
-        <v>10</v>
-      </c>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="10">
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a__x000a_You can enter a maximum of 30 characters._x000a__x000a_Select Cancel and enter the details again._x000a_" sqref="A2:C30" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a__x000a_The value entered must not exceed 99999999.99. _x000a__x000a_Select Cancel and enter the details again._x000a_" sqref="G1">
+      <formula1>1</formula1>
+      <formula2>99999999999</formula2>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a_You can enter a maximum of 12 characters._x000a_Select Cancel and enter the details again._x000a_" sqref="I1">
+      <formula1>1</formula1>
+      <formula2>12</formula2>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a__x000a_You can enter a maximum of 30 characters._x000a__x000a_Select Cancel and enter the details again._x000a_" sqref="A2:C21">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a__x000a_The date must be entered as DD/MM/YYYY._x000a__x000a_Select Cancel and enter the details again._x000a_" sqref="D2:D30" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a__x000a_The date must be entered as DD/MM/YYYY._x000a__x000a_Select Cancel and enter the details again._x000a_" sqref="D2:D21">
       <formula1>29221</formula1>
       <formula2>73050</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a__x000a_You can enter a maximum of 12 characters._x000a__x000a_Select Cancel and enter the details again._x000a_" sqref="I2:I30" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a__x000a_You can enter a maximum of 12 characters._x000a__x000a_Select Cancel and enter the details again._x000a_" sqref="I2:I21">
       <formula1>1</formula1>
       <formula2>12</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a__x000a_The value entered must not exceed 99999999.99. _x000a__x000a_Select Cancel and enter the details again._x000a_" sqref="G1" xr:uid="{00000000-0002-0000-0000-000003000000}">
-      <formula1>1</formula1>
-      <formula2>99999999999</formula2>
-    </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a_You can enter a maximum of 12 characters._x000a_Select Cancel and enter the details again._x000a_" sqref="I1" xr:uid="{00000000-0002-0000-0000-000004000000}">
-      <formula1>1</formula1>
-      <formula2>12</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a__x000a_The value entered must not exceed 99999999.99. _x000a__x000a_Select Cancel and enter the details again._x000a_" sqref="G2:G30" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a__x000a_The value entered must not exceed 99999999.99. _x000a__x000a_Select Cancel and enter the details again._x000a_" sqref="G2:G21">
       <formula1>0.000001</formula1>
       <formula2>99999999.99</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a__x000a_You can enter a maximum of 8 characters._x000a__x000a_Select Cancel and enter the details again._x000a_" sqref="J2:J30" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a__x000a_You can enter a maximum of 8 characters._x000a__x000a_Select Cancel and enter the details again._x000a_" sqref="J2:J21">
       <formula1>1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a__x000a_You can enter a maximum of 60 characters._x000a__x000a_Select Cancel and enter the details again._x000a_" sqref="F2:F30" xr:uid="{00000000-0002-0000-0000-000008000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a__x000a_You can enter a maximum of 60 characters._x000a__x000a_Select Cancel and enter the details again._x000a_" sqref="F2:F21">
       <formula1>1</formula1>
       <formula2>60</formula2>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a_You can enter a maximum of 30 characters._x000a_Select Cancel and enter the details again._x000a_" sqref="E2:E30" xr:uid="{00000000-0002-0000-0000-000009000000}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a_You can enter a maximum of 30 characters._x000a_Select Cancel and enter the details again._x000a_" sqref="E2:E21">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a__x000a_The value entered must not exceed 99999999.99. _x000a__x000a_Select Cancel and enter the details again._x000a_" sqref="H2:H30" xr:uid="{00000000-0002-0000-0000-00000A000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Error!" error="The information you have entered is incorrect._x000a__x000a_The value entered must not exceed 99999999.99. _x000a__x000a_Select Cancel and enter the details again._x000a_" sqref="H2:H21">
       <formula1>0</formula1>
       <formula2>99999999.99</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="E14" numberStoredAsText="1"/>
-  </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>